<commit_message>
another local repo push
</commit_message>
<xml_diff>
--- a/test/a.xlsx
+++ b/test/a.xlsx
@@ -341,7 +341,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -351,11 +351,11 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1">
-        <f>SUM(A1:B1)</f>
-        <v>7</v>
+        <f>SUM(A1:B1)+1</f>
+        <v>10</v>
       </c>
       <c r="D1">
         <v>4</v>

</xml_diff>